<commit_message>
send files to s3
</commit_message>
<xml_diff>
--- a/server/pyreport/report.xlsx
+++ b/server/pyreport/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wwl_dashboard\server\pyreport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F206F-371E-4644-A704-E6EA44354D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{48F9245D-8BA6-4F3B-8254-7482C1827B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F55265A8-C2C8-4C42-8CBD-B0824D47FF9B}"/>
   </bookViews>
@@ -167,7 +167,7 @@
     <numFmt numFmtId="165" formatCode="[$-409]mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +265,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -703,7 +709,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
@@ -801,13 +807,52 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -817,18 +862,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,33 +888,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="32" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma 3 2" xfId="8" xr:uid="{ED1C13C5-4918-4F9F-A9C4-6EB536AA41AC}"/>
@@ -4112,12 +4119,12 @@
     <tabColor indexed="10"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W82"/>
+  <dimension ref="A1:Y88"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M160" sqref="M160"/>
-      <selection pane="bottomLeft" activeCell="U84" sqref="U84"/>
+      <selection pane="bottomLeft" activeCell="Y85" sqref="Y85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4154,26 +4161,26 @@
     </row>
     <row r="2" spans="1:23" ht="10.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="61"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
+      <c r="U2" s="70"/>
     </row>
     <row r="3" spans="1:23" s="10" customFormat="1" ht="40.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -4181,15 +4188,15 @@
         <v>0</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
       <c r="K3" s="7" t="s">
         <v>1</v>
       </c>
@@ -4220,9 +4227,9 @@
       <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="13"/>
@@ -4243,38 +4250,38 @@
         <v>3</v>
       </c>
       <c r="L5" s="8"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
+      <c r="M5" s="73"/>
+      <c r="N5" s="73"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="73"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="9"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="66"/>
+      <c r="S5" s="74"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="75"/>
     </row>
     <row r="6" spans="1:23" ht="6.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="68"/>
-      <c r="P6" s="68"/>
-      <c r="Q6" s="68"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="68"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="69"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="58"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="59"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
@@ -4370,21 +4377,21 @@
     <row r="11" spans="1:23" ht="31.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
-      <c r="G11" s="52" t="s">
+      <c r="G11" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="52" t="s">
+      <c r="H11" s="66"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="53"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="52" t="s">
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="53"/>
-      <c r="O11" s="54"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="67"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="33"/>
@@ -4395,33 +4402,33 @@
     <row r="12" spans="1:23" s="26" customFormat="1" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="35"/>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="51"/>
-      <c r="E12" s="49" t="s">
+      <c r="D12" s="61"/>
+      <c r="E12" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="51"/>
-      <c r="G12" s="49" t="s">
+      <c r="F12" s="61"/>
+      <c r="G12" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="50"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="49" t="s">
+      <c r="H12" s="64"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="50"/>
-      <c r="L12" s="51"/>
-      <c r="M12" s="49" t="s">
+      <c r="K12" s="64"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
-      <c r="P12" s="49" t="s">
+      <c r="N12" s="64"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="51"/>
+      <c r="Q12" s="61"/>
       <c r="R12" s="33"/>
       <c r="S12" s="33"/>
       <c r="T12" s="33"/>
@@ -4430,10 +4437,10 @@
     <row r="13" spans="1:23" s="31" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="27"/>
       <c r="B13" s="28"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="63"/>
       <c r="G13" s="29" t="s">
         <v>9</v>
       </c>
@@ -4461,8 +4468,8 @@
       <c r="O13" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="56"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="63"/>
       <c r="R13" s="33"/>
       <c r="S13" s="33"/>
       <c r="T13" s="33"/>
@@ -4471,10 +4478,10 @@
     <row r="14" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="58"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
       <c r="G14" s="41"/>
       <c r="H14" s="42"/>
       <c r="I14" s="43"/>
@@ -4484,8 +4491,8 @@
       <c r="M14" s="41"/>
       <c r="N14" s="42"/>
       <c r="O14" s="43"/>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="71"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="54"/>
       <c r="R14" s="33"/>
       <c r="S14" s="33"/>
       <c r="T14" s="33"/>
@@ -4495,10 +4502,10 @@
     <row r="15" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
       <c r="G15" s="44"/>
       <c r="H15" s="42"/>
       <c r="I15" s="45"/>
@@ -4508,8 +4515,8 @@
       <c r="M15" s="44"/>
       <c r="N15" s="42"/>
       <c r="O15" s="45"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="71"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="54"/>
       <c r="R15" s="33"/>
       <c r="S15" s="33"/>
       <c r="T15" s="33"/>
@@ -4519,10 +4526,10 @@
     <row r="16" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="16"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="44"/>
       <c r="H16" s="42"/>
       <c r="I16" s="45"/>
@@ -4532,8 +4539,8 @@
       <c r="M16" s="44"/>
       <c r="N16" s="42"/>
       <c r="O16" s="45"/>
-      <c r="P16" s="70"/>
-      <c r="Q16" s="71"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="54"/>
       <c r="R16" s="33"/>
       <c r="S16" s="33"/>
       <c r="T16" s="33"/>
@@ -4543,10 +4550,10 @@
     <row r="17" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="16"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="44"/>
       <c r="H17" s="42"/>
       <c r="I17" s="45"/>
@@ -4556,8 +4563,8 @@
       <c r="M17" s="44"/>
       <c r="N17" s="42"/>
       <c r="O17" s="45"/>
-      <c r="P17" s="70"/>
-      <c r="Q17" s="71"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="54"/>
       <c r="R17" s="33"/>
       <c r="S17" s="33"/>
       <c r="T17" s="33"/>
@@ -4567,10 +4574,10 @@
     <row r="18" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="58"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="44"/>
       <c r="H18" s="42"/>
       <c r="I18" s="45"/>
@@ -4580,8 +4587,8 @@
       <c r="M18" s="44"/>
       <c r="N18" s="42"/>
       <c r="O18" s="45"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="71"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="54"/>
       <c r="R18" s="33"/>
       <c r="S18" s="33"/>
       <c r="T18" s="33"/>
@@ -4591,10 +4598,10 @@
     <row r="19" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="16"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="44"/>
       <c r="H19" s="42"/>
       <c r="I19" s="45"/>
@@ -4604,8 +4611,8 @@
       <c r="M19" s="44"/>
       <c r="N19" s="42"/>
       <c r="O19" s="45"/>
-      <c r="P19" s="70"/>
-      <c r="Q19" s="71"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="54"/>
       <c r="R19" s="33"/>
       <c r="S19" s="33"/>
       <c r="T19" s="33"/>
@@ -4615,10 +4622,10 @@
     <row r="20" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="58"/>
+      <c r="C20" s="55"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="56"/>
       <c r="G20" s="44"/>
       <c r="H20" s="42"/>
       <c r="I20" s="45"/>
@@ -4628,8 +4635,8 @@
       <c r="M20" s="44"/>
       <c r="N20" s="42"/>
       <c r="O20" s="45"/>
-      <c r="P20" s="70"/>
-      <c r="Q20" s="71"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="54"/>
       <c r="R20" s="33"/>
       <c r="S20" s="33"/>
       <c r="T20" s="33"/>
@@ -4639,10 +4646,10 @@
     <row r="21" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="16"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="58"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="58"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
       <c r="G21" s="44"/>
       <c r="H21" s="42"/>
       <c r="I21" s="45"/>
@@ -4652,8 +4659,8 @@
       <c r="M21" s="44"/>
       <c r="N21" s="42"/>
       <c r="O21" s="45"/>
-      <c r="P21" s="70"/>
-      <c r="Q21" s="71"/>
+      <c r="P21" s="53"/>
+      <c r="Q21" s="54"/>
       <c r="R21" s="33"/>
       <c r="S21" s="33"/>
       <c r="T21" s="33"/>
@@ -4663,10 +4670,10 @@
     <row r="22" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="16"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="58"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="44"/>
       <c r="H22" s="42"/>
       <c r="I22" s="45"/>
@@ -4676,8 +4683,8 @@
       <c r="M22" s="44"/>
       <c r="N22" s="42"/>
       <c r="O22" s="45"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="71"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="54"/>
       <c r="R22" s="33"/>
       <c r="S22" s="33"/>
       <c r="T22" s="33"/>
@@ -4687,10 +4694,10 @@
     <row r="23" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="56"/>
       <c r="G23" s="44"/>
       <c r="H23" s="42"/>
       <c r="I23" s="45"/>
@@ -4700,8 +4707,8 @@
       <c r="M23" s="44"/>
       <c r="N23" s="42"/>
       <c r="O23" s="45"/>
-      <c r="P23" s="70"/>
-      <c r="Q23" s="71"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="54"/>
       <c r="R23" s="33"/>
       <c r="S23" s="33"/>
       <c r="T23" s="33"/>
@@ -4711,10 +4718,10 @@
     <row r="24" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="58"/>
+      <c r="C24" s="55"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="56"/>
       <c r="G24" s="44"/>
       <c r="H24" s="42"/>
       <c r="I24" s="45"/>
@@ -4724,8 +4731,8 @@
       <c r="M24" s="44"/>
       <c r="N24" s="42"/>
       <c r="O24" s="45"/>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="71"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="54"/>
       <c r="R24" s="33"/>
       <c r="S24" s="33"/>
       <c r="T24" s="33"/>
@@ -4735,10 +4742,10 @@
     <row r="25" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="58"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="44"/>
       <c r="H25" s="42"/>
       <c r="I25" s="45"/>
@@ -4748,8 +4755,8 @@
       <c r="M25" s="44"/>
       <c r="N25" s="42"/>
       <c r="O25" s="45"/>
-      <c r="P25" s="70"/>
-      <c r="Q25" s="71"/>
+      <c r="P25" s="53"/>
+      <c r="Q25" s="54"/>
       <c r="R25" s="33"/>
       <c r="S25" s="33"/>
       <c r="T25" s="33"/>
@@ -4759,10 +4766,10 @@
     <row r="26" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="56"/>
       <c r="G26" s="44"/>
       <c r="H26" s="42"/>
       <c r="I26" s="45"/>
@@ -4772,8 +4779,8 @@
       <c r="M26" s="44"/>
       <c r="N26" s="42"/>
       <c r="O26" s="45"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="71"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="54"/>
       <c r="R26" s="33"/>
       <c r="S26" s="33"/>
       <c r="T26" s="33"/>
@@ -4783,10 +4790,10 @@
     <row r="27" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="56"/>
       <c r="G27" s="44"/>
       <c r="H27" s="42"/>
       <c r="I27" s="45"/>
@@ -4796,8 +4803,8 @@
       <c r="M27" s="44"/>
       <c r="N27" s="42"/>
       <c r="O27" s="45"/>
-      <c r="P27" s="70"/>
-      <c r="Q27" s="71"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="54"/>
       <c r="R27" s="33"/>
       <c r="S27" s="33"/>
       <c r="T27" s="33"/>
@@ -4807,10 +4814,10 @@
     <row r="28" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="58"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="44"/>
       <c r="H28" s="42"/>
       <c r="I28" s="45"/>
@@ -4820,8 +4827,8 @@
       <c r="M28" s="44"/>
       <c r="N28" s="42"/>
       <c r="O28" s="45"/>
-      <c r="P28" s="70"/>
-      <c r="Q28" s="71"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="54"/>
       <c r="R28" s="33"/>
       <c r="S28" s="33"/>
       <c r="T28" s="33"/>
@@ -4831,10 +4838,10 @@
     <row r="29" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3"/>
       <c r="B29" s="16"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="56"/>
       <c r="G29" s="44"/>
       <c r="H29" s="42"/>
       <c r="I29" s="45"/>
@@ -4844,8 +4851,8 @@
       <c r="M29" s="44"/>
       <c r="N29" s="42"/>
       <c r="O29" s="45"/>
-      <c r="P29" s="70"/>
-      <c r="Q29" s="71"/>
+      <c r="P29" s="53"/>
+      <c r="Q29" s="54"/>
       <c r="R29" s="33"/>
       <c r="S29" s="33"/>
       <c r="T29" s="33"/>
@@ -4855,10 +4862,10 @@
     <row r="30" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3"/>
       <c r="B30" s="16"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="58"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="56"/>
       <c r="G30" s="44"/>
       <c r="H30" s="42"/>
       <c r="I30" s="45"/>
@@ -4868,8 +4875,8 @@
       <c r="M30" s="44"/>
       <c r="N30" s="42"/>
       <c r="O30" s="45"/>
-      <c r="P30" s="70"/>
-      <c r="Q30" s="71"/>
+      <c r="P30" s="53"/>
+      <c r="Q30" s="54"/>
       <c r="R30" s="33"/>
       <c r="S30" s="33"/>
       <c r="T30" s="33"/>
@@ -4879,10 +4886,10 @@
     <row r="31" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3"/>
       <c r="B31" s="16"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="58"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="44"/>
       <c r="H31" s="42"/>
       <c r="I31" s="45"/>
@@ -4892,8 +4899,8 @@
       <c r="M31" s="44"/>
       <c r="N31" s="42"/>
       <c r="O31" s="45"/>
-      <c r="P31" s="70"/>
-      <c r="Q31" s="71"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="54"/>
       <c r="R31" s="33"/>
       <c r="S31" s="33"/>
       <c r="T31" s="33"/>
@@ -4903,10 +4910,10 @@
     <row r="32" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3"/>
       <c r="B32" s="16"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="58"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="44"/>
       <c r="H32" s="42"/>
       <c r="I32" s="45"/>
@@ -4916,8 +4923,8 @@
       <c r="M32" s="44"/>
       <c r="N32" s="42"/>
       <c r="O32" s="45"/>
-      <c r="P32" s="70"/>
-      <c r="Q32" s="71"/>
+      <c r="P32" s="53"/>
+      <c r="Q32" s="54"/>
       <c r="R32" s="33"/>
       <c r="S32" s="33"/>
       <c r="T32" s="33"/>
@@ -4927,10 +4934,10 @@
     <row r="33" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="56"/>
       <c r="G33" s="44"/>
       <c r="H33" s="42"/>
       <c r="I33" s="45"/>
@@ -4940,8 +4947,8 @@
       <c r="M33" s="44"/>
       <c r="N33" s="42"/>
       <c r="O33" s="45"/>
-      <c r="P33" s="70"/>
-      <c r="Q33" s="71"/>
+      <c r="P33" s="53"/>
+      <c r="Q33" s="54"/>
       <c r="R33" s="33"/>
       <c r="S33" s="33"/>
       <c r="T33" s="33"/>
@@ -4951,10 +4958,10 @@
     <row r="34" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="58"/>
+      <c r="C34" s="55"/>
+      <c r="D34" s="56"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="56"/>
       <c r="G34" s="44"/>
       <c r="H34" s="42"/>
       <c r="I34" s="45"/>
@@ -4964,8 +4971,8 @@
       <c r="M34" s="44"/>
       <c r="N34" s="42"/>
       <c r="O34" s="45"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="71"/>
+      <c r="P34" s="53"/>
+      <c r="Q34" s="54"/>
       <c r="R34" s="33"/>
       <c r="S34" s="33"/>
       <c r="T34" s="33"/>
@@ -4975,10 +4982,10 @@
     <row r="35" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
       <c r="B35" s="16"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="57"/>
-      <c r="F35" s="58"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="56"/>
       <c r="G35" s="44"/>
       <c r="H35" s="42"/>
       <c r="I35" s="45"/>
@@ -4988,8 +4995,8 @@
       <c r="M35" s="44"/>
       <c r="N35" s="42"/>
       <c r="O35" s="45"/>
-      <c r="P35" s="70"/>
-      <c r="Q35" s="71"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="54"/>
       <c r="R35" s="33"/>
       <c r="S35" s="33"/>
       <c r="T35" s="33"/>
@@ -4999,10 +5006,10 @@
     <row r="36" spans="1:23" s="32" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3"/>
       <c r="B36" s="16"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="57"/>
-      <c r="F36" s="58"/>
+      <c r="C36" s="55"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="56"/>
       <c r="G36" s="44"/>
       <c r="H36" s="42"/>
       <c r="I36" s="45"/>
@@ -5012,8 +5019,8 @@
       <c r="M36" s="44"/>
       <c r="N36" s="42"/>
       <c r="O36" s="45"/>
-      <c r="P36" s="70"/>
-      <c r="Q36" s="71"/>
+      <c r="P36" s="53"/>
+      <c r="Q36" s="54"/>
       <c r="R36" s="33"/>
       <c r="S36" s="33"/>
       <c r="T36" s="33"/>
@@ -5023,10 +5030,10 @@
     <row r="37" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3"/>
       <c r="B37" s="16"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="58"/>
+      <c r="C37" s="55"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="55"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="44"/>
       <c r="H37" s="42"/>
       <c r="I37" s="45"/>
@@ -5036,8 +5043,8 @@
       <c r="M37" s="44"/>
       <c r="N37" s="42"/>
       <c r="O37" s="45"/>
-      <c r="P37" s="70"/>
-      <c r="Q37" s="71"/>
+      <c r="P37" s="53"/>
+      <c r="Q37" s="54"/>
       <c r="R37" s="33"/>
       <c r="S37" s="33"/>
       <c r="T37" s="33"/>
@@ -5046,10 +5053,10 @@
     <row r="38" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="16"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="58"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="44"/>
       <c r="H38" s="42"/>
       <c r="I38" s="45"/>
@@ -5059,8 +5066,8 @@
       <c r="M38" s="44"/>
       <c r="N38" s="42"/>
       <c r="O38" s="45"/>
-      <c r="P38" s="70"/>
-      <c r="Q38" s="71"/>
+      <c r="P38" s="53"/>
+      <c r="Q38" s="54"/>
       <c r="R38" s="33"/>
       <c r="S38" s="33"/>
       <c r="T38" s="33"/>
@@ -5069,10 +5076,10 @@
     <row r="39" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="16"/>
-      <c r="C39" s="57"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="57"/>
-      <c r="F39" s="58"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="56"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="44"/>
       <c r="H39" s="42"/>
       <c r="I39" s="45"/>
@@ -5082,8 +5089,8 @@
       <c r="M39" s="44"/>
       <c r="N39" s="42"/>
       <c r="O39" s="45"/>
-      <c r="P39" s="70"/>
-      <c r="Q39" s="71"/>
+      <c r="P39" s="53"/>
+      <c r="Q39" s="54"/>
       <c r="R39" s="33"/>
       <c r="S39" s="33"/>
       <c r="T39" s="33"/>
@@ -5091,10 +5098,10 @@
     </row>
     <row r="40" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="16"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="56"/>
       <c r="G40" s="44"/>
       <c r="H40" s="42"/>
       <c r="I40" s="45"/>
@@ -5104,8 +5111,8 @@
       <c r="M40" s="44"/>
       <c r="N40" s="42"/>
       <c r="O40" s="45"/>
-      <c r="P40" s="70"/>
-      <c r="Q40" s="71"/>
+      <c r="P40" s="53"/>
+      <c r="Q40" s="54"/>
       <c r="R40" s="33"/>
       <c r="S40" s="33"/>
       <c r="T40" s="33"/>
@@ -5116,10 +5123,10 @@
     <row r="41" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3"/>
       <c r="B41" s="16"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="56"/>
       <c r="G41" s="44"/>
       <c r="H41" s="42"/>
       <c r="I41" s="45"/>
@@ -5129,8 +5136,8 @@
       <c r="M41" s="44"/>
       <c r="N41" s="42"/>
       <c r="O41" s="45"/>
-      <c r="P41" s="70"/>
-      <c r="Q41" s="71"/>
+      <c r="P41" s="53"/>
+      <c r="Q41" s="54"/>
       <c r="R41" s="33"/>
       <c r="S41" s="33"/>
       <c r="T41" s="33"/>
@@ -5141,10 +5148,10 @@
     <row r="42" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
       <c r="B42" s="16"/>
-      <c r="C42" s="57"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="57"/>
-      <c r="F42" s="58"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="55"/>
+      <c r="F42" s="56"/>
       <c r="G42" s="44"/>
       <c r="H42" s="42"/>
       <c r="I42" s="45"/>
@@ -5154,8 +5161,8 @@
       <c r="M42" s="44"/>
       <c r="N42" s="42"/>
       <c r="O42" s="45"/>
-      <c r="P42" s="70"/>
-      <c r="Q42" s="71"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="54"/>
       <c r="R42" s="33"/>
       <c r="S42" s="33"/>
       <c r="T42" s="33"/>
@@ -5166,10 +5173,10 @@
     <row r="43" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
       <c r="B43" s="16"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="58"/>
+      <c r="C43" s="55"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="55"/>
+      <c r="F43" s="56"/>
       <c r="G43" s="44"/>
       <c r="H43" s="42"/>
       <c r="I43" s="45"/>
@@ -5179,8 +5186,8 @@
       <c r="M43" s="44"/>
       <c r="N43" s="42"/>
       <c r="O43" s="45"/>
-      <c r="P43" s="70"/>
-      <c r="Q43" s="71"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="54"/>
       <c r="R43" s="33"/>
       <c r="S43" s="33"/>
       <c r="T43" s="33"/>
@@ -5189,10 +5196,10 @@
     <row r="44" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="16"/>
-      <c r="C44" s="57"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="56"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="56"/>
       <c r="G44" s="44"/>
       <c r="H44" s="42"/>
       <c r="I44" s="45"/>
@@ -5202,8 +5209,8 @@
       <c r="M44" s="44"/>
       <c r="N44" s="42"/>
       <c r="O44" s="45"/>
-      <c r="P44" s="70"/>
-      <c r="Q44" s="71"/>
+      <c r="P44" s="53"/>
+      <c r="Q44" s="54"/>
       <c r="R44" s="33"/>
       <c r="S44" s="33"/>
       <c r="T44" s="33"/>
@@ -5212,10 +5219,10 @@
     <row r="45" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
       <c r="B45" s="16"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="58"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="56"/>
       <c r="G45" s="44"/>
       <c r="H45" s="42"/>
       <c r="I45" s="45"/>
@@ -5225,8 +5232,8 @@
       <c r="M45" s="44"/>
       <c r="N45" s="42"/>
       <c r="O45" s="45"/>
-      <c r="P45" s="70"/>
-      <c r="Q45" s="71"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="54"/>
       <c r="R45" s="33"/>
       <c r="S45" s="33"/>
       <c r="T45" s="33"/>
@@ -5235,10 +5242,10 @@
     <row r="46" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3"/>
       <c r="B46" s="16"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="56"/>
       <c r="G46" s="44"/>
       <c r="H46" s="42"/>
       <c r="I46" s="45"/>
@@ -5248,8 +5255,8 @@
       <c r="M46" s="44"/>
       <c r="N46" s="42"/>
       <c r="O46" s="45"/>
-      <c r="P46" s="70"/>
-      <c r="Q46" s="71"/>
+      <c r="P46" s="53"/>
+      <c r="Q46" s="54"/>
       <c r="R46" s="33"/>
       <c r="S46" s="33"/>
       <c r="T46" s="33"/>
@@ -5258,10 +5265,10 @@
     <row r="47" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3"/>
       <c r="B47" s="16"/>
-      <c r="C47" s="57"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="56"/>
       <c r="G47" s="44"/>
       <c r="H47" s="42"/>
       <c r="I47" s="45"/>
@@ -5271,8 +5278,8 @@
       <c r="M47" s="44"/>
       <c r="N47" s="42"/>
       <c r="O47" s="45"/>
-      <c r="P47" s="70"/>
-      <c r="Q47" s="71"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="54"/>
       <c r="R47" s="33"/>
       <c r="S47" s="33"/>
       <c r="T47" s="33"/>
@@ -5281,10 +5288,10 @@
     <row r="48" spans="1:23" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="16"/>
-      <c r="C48" s="57"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="56"/>
       <c r="G48" s="44"/>
       <c r="H48" s="42"/>
       <c r="I48" s="45"/>
@@ -5294,8 +5301,8 @@
       <c r="M48" s="44"/>
       <c r="N48" s="42"/>
       <c r="O48" s="45"/>
-      <c r="P48" s="70"/>
-      <c r="Q48" s="71"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="54"/>
       <c r="R48" s="33"/>
       <c r="S48" s="33"/>
       <c r="T48" s="33"/>
@@ -5304,10 +5311,10 @@
     <row r="49" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="16"/>
-      <c r="C49" s="57"/>
-      <c r="D49" s="58"/>
-      <c r="E49" s="57"/>
-      <c r="F49" s="58"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="55"/>
+      <c r="F49" s="56"/>
       <c r="G49" s="44"/>
       <c r="H49" s="42"/>
       <c r="I49" s="45"/>
@@ -5317,8 +5324,8 @@
       <c r="M49" s="44"/>
       <c r="N49" s="42"/>
       <c r="O49" s="45"/>
-      <c r="P49" s="70"/>
-      <c r="Q49" s="71"/>
+      <c r="P49" s="53"/>
+      <c r="Q49" s="54"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
@@ -5327,10 +5334,10 @@
     <row r="50" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34"/>
       <c r="B50" s="16"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="58"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="56"/>
       <c r="G50" s="44"/>
       <c r="H50" s="42"/>
       <c r="I50" s="45"/>
@@ -5340,8 +5347,8 @@
       <c r="M50" s="44"/>
       <c r="N50" s="42"/>
       <c r="O50" s="45"/>
-      <c r="P50" s="70"/>
-      <c r="Q50" s="71"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="54"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
@@ -5350,10 +5357,10 @@
     <row r="51" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="16"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="55"/>
+      <c r="F51" s="56"/>
       <c r="G51" s="44"/>
       <c r="H51" s="42"/>
       <c r="I51" s="45"/>
@@ -5363,8 +5370,8 @@
       <c r="M51" s="44"/>
       <c r="N51" s="42"/>
       <c r="O51" s="45"/>
-      <c r="P51" s="70"/>
-      <c r="Q51" s="71"/>
+      <c r="P51" s="53"/>
+      <c r="Q51" s="54"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
@@ -5373,10 +5380,10 @@
     <row r="52" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="16"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="58"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="58"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="56"/>
       <c r="G52" s="44"/>
       <c r="H52" s="42"/>
       <c r="I52" s="45"/>
@@ -5386,8 +5393,8 @@
       <c r="M52" s="44"/>
       <c r="N52" s="42"/>
       <c r="O52" s="45"/>
-      <c r="P52" s="70"/>
-      <c r="Q52" s="71"/>
+      <c r="P52" s="53"/>
+      <c r="Q52" s="54"/>
       <c r="R52" s="1"/>
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
@@ -5395,10 +5402,10 @@
     </row>
     <row r="53" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="16"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="56"/>
       <c r="G53" s="44"/>
       <c r="H53" s="42"/>
       <c r="I53" s="45"/>
@@ -5408,8 +5415,8 @@
       <c r="M53" s="44"/>
       <c r="N53" s="42"/>
       <c r="O53" s="45"/>
-      <c r="P53" s="70"/>
-      <c r="Q53" s="71"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="54"/>
       <c r="R53" s="1"/>
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
@@ -5417,10 +5424,10 @@
     </row>
     <row r="54" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="16"/>
-      <c r="C54" s="57"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="57"/>
-      <c r="F54" s="58"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="55"/>
+      <c r="F54" s="56"/>
       <c r="G54" s="44"/>
       <c r="H54" s="42"/>
       <c r="I54" s="45"/>
@@ -5430,8 +5437,8 @@
       <c r="M54" s="44"/>
       <c r="N54" s="42"/>
       <c r="O54" s="45"/>
-      <c r="P54" s="70"/>
-      <c r="Q54" s="71"/>
+      <c r="P54" s="53"/>
+      <c r="Q54" s="54"/>
       <c r="R54" s="1"/>
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
@@ -5439,10 +5446,10 @@
     </row>
     <row r="55" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="16"/>
-      <c r="C55" s="57"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="57"/>
-      <c r="F55" s="58"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="55"/>
+      <c r="F55" s="56"/>
       <c r="G55" s="44"/>
       <c r="H55" s="42"/>
       <c r="I55" s="45"/>
@@ -5452,8 +5459,8 @@
       <c r="M55" s="44"/>
       <c r="N55" s="42"/>
       <c r="O55" s="45"/>
-      <c r="P55" s="70"/>
-      <c r="Q55" s="71"/>
+      <c r="P55" s="53"/>
+      <c r="Q55" s="54"/>
       <c r="R55" s="1"/>
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
@@ -5461,10 +5468,10 @@
     </row>
     <row r="56" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="16"/>
-      <c r="C56" s="57"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="57"/>
-      <c r="F56" s="58"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="56"/>
       <c r="G56" s="44"/>
       <c r="H56" s="42"/>
       <c r="I56" s="45"/>
@@ -5474,8 +5481,8 @@
       <c r="M56" s="44"/>
       <c r="N56" s="42"/>
       <c r="O56" s="45"/>
-      <c r="P56" s="70"/>
-      <c r="Q56" s="71"/>
+      <c r="P56" s="53"/>
+      <c r="Q56" s="54"/>
       <c r="R56" s="1"/>
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
@@ -5483,10 +5490,10 @@
     </row>
     <row r="57" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="16"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="57"/>
-      <c r="F57" s="58"/>
+      <c r="C57" s="55"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="55"/>
+      <c r="F57" s="56"/>
       <c r="G57" s="44"/>
       <c r="H57" s="42"/>
       <c r="I57" s="45"/>
@@ -5496,8 +5503,8 @@
       <c r="M57" s="44"/>
       <c r="N57" s="42"/>
       <c r="O57" s="45"/>
-      <c r="P57" s="70"/>
-      <c r="Q57" s="71"/>
+      <c r="P57" s="53"/>
+      <c r="Q57" s="54"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
@@ -5505,10 +5512,10 @@
     </row>
     <row r="58" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="16"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="57"/>
-      <c r="F58" s="58"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="56"/>
       <c r="G58" s="44"/>
       <c r="H58" s="42"/>
       <c r="I58" s="45"/>
@@ -5518,8 +5525,8 @@
       <c r="M58" s="44"/>
       <c r="N58" s="42"/>
       <c r="O58" s="45"/>
-      <c r="P58" s="70"/>
-      <c r="Q58" s="71"/>
+      <c r="P58" s="53"/>
+      <c r="Q58" s="54"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
@@ -5527,10 +5534,10 @@
     </row>
     <row r="59" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="16"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="57"/>
-      <c r="F59" s="58"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="56"/>
+      <c r="E59" s="55"/>
+      <c r="F59" s="56"/>
       <c r="G59" s="44"/>
       <c r="H59" s="42"/>
       <c r="I59" s="45"/>
@@ -5540,8 +5547,8 @@
       <c r="M59" s="44"/>
       <c r="N59" s="42"/>
       <c r="O59" s="45"/>
-      <c r="P59" s="70"/>
-      <c r="Q59" s="71"/>
+      <c r="P59" s="53"/>
+      <c r="Q59" s="54"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
@@ -5549,10 +5556,10 @@
     </row>
     <row r="60" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="16"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="58"/>
+      <c r="C60" s="55"/>
+      <c r="D60" s="56"/>
+      <c r="E60" s="55"/>
+      <c r="F60" s="56"/>
       <c r="G60" s="44"/>
       <c r="H60" s="42"/>
       <c r="I60" s="45"/>
@@ -5562,8 +5569,8 @@
       <c r="M60" s="44"/>
       <c r="N60" s="42"/>
       <c r="O60" s="45"/>
-      <c r="P60" s="70"/>
-      <c r="Q60" s="71"/>
+      <c r="P60" s="53"/>
+      <c r="Q60" s="54"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
@@ -5571,10 +5578,10 @@
     </row>
     <row r="61" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="16"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="58"/>
+      <c r="C61" s="55"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="56"/>
       <c r="G61" s="44"/>
       <c r="H61" s="42"/>
       <c r="I61" s="45"/>
@@ -5584,8 +5591,8 @@
       <c r="M61" s="44"/>
       <c r="N61" s="42"/>
       <c r="O61" s="45"/>
-      <c r="P61" s="70"/>
-      <c r="Q61" s="71"/>
+      <c r="P61" s="53"/>
+      <c r="Q61" s="54"/>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
@@ -5593,10 +5600,10 @@
     </row>
     <row r="62" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="16"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="57"/>
-      <c r="F62" s="58"/>
+      <c r="C62" s="55"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="55"/>
+      <c r="F62" s="56"/>
       <c r="G62" s="44"/>
       <c r="H62" s="42"/>
       <c r="I62" s="45"/>
@@ -5606,8 +5613,8 @@
       <c r="M62" s="44"/>
       <c r="N62" s="42"/>
       <c r="O62" s="45"/>
-      <c r="P62" s="70"/>
-      <c r="Q62" s="71"/>
+      <c r="P62" s="53"/>
+      <c r="Q62" s="54"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
@@ -5615,10 +5622,10 @@
     </row>
     <row r="63" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="16"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="57"/>
-      <c r="F63" s="58"/>
+      <c r="C63" s="55"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="55"/>
+      <c r="F63" s="56"/>
       <c r="G63" s="44"/>
       <c r="H63" s="42"/>
       <c r="I63" s="45"/>
@@ -5628,8 +5635,8 @@
       <c r="M63" s="44"/>
       <c r="N63" s="42"/>
       <c r="O63" s="45"/>
-      <c r="P63" s="70"/>
-      <c r="Q63" s="71"/>
+      <c r="P63" s="53"/>
+      <c r="Q63" s="54"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
@@ -5637,10 +5644,10 @@
     </row>
     <row r="64" spans="1:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="16"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="58"/>
+      <c r="C64" s="55"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="55"/>
+      <c r="F64" s="56"/>
       <c r="G64" s="44"/>
       <c r="H64" s="42"/>
       <c r="I64" s="45"/>
@@ -5650,8 +5657,8 @@
       <c r="M64" s="44"/>
       <c r="N64" s="42"/>
       <c r="O64" s="45"/>
-      <c r="P64" s="70"/>
-      <c r="Q64" s="71"/>
+      <c r="P64" s="53"/>
+      <c r="Q64" s="54"/>
       <c r="R64" s="1"/>
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
@@ -5659,10 +5666,10 @@
     </row>
     <row r="65" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="16"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="58"/>
+      <c r="C65" s="55"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="55"/>
+      <c r="F65" s="56"/>
       <c r="G65" s="44"/>
       <c r="H65" s="42"/>
       <c r="I65" s="45"/>
@@ -5672,8 +5679,8 @@
       <c r="M65" s="44"/>
       <c r="N65" s="42"/>
       <c r="O65" s="45"/>
-      <c r="P65" s="70"/>
-      <c r="Q65" s="71"/>
+      <c r="P65" s="53"/>
+      <c r="Q65" s="54"/>
       <c r="R65" s="1"/>
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
@@ -5681,10 +5688,10 @@
     </row>
     <row r="66" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="16"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="57"/>
-      <c r="F66" s="58"/>
+      <c r="C66" s="55"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="56"/>
       <c r="G66" s="44"/>
       <c r="H66" s="42"/>
       <c r="I66" s="45"/>
@@ -5694,8 +5701,8 @@
       <c r="M66" s="44"/>
       <c r="N66" s="42"/>
       <c r="O66" s="45"/>
-      <c r="P66" s="70"/>
-      <c r="Q66" s="71"/>
+      <c r="P66" s="53"/>
+      <c r="Q66" s="54"/>
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
@@ -5703,10 +5710,10 @@
     </row>
     <row r="67" spans="2:21" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="16"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="57"/>
-      <c r="F67" s="58"/>
+      <c r="C67" s="55"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="56"/>
       <c r="G67" s="44"/>
       <c r="H67" s="42"/>
       <c r="I67" s="45"/>
@@ -5716,8 +5723,8 @@
       <c r="M67" s="44"/>
       <c r="N67" s="42"/>
       <c r="O67" s="45"/>
-      <c r="P67" s="70"/>
-      <c r="Q67" s="71"/>
+      <c r="P67" s="53"/>
+      <c r="Q67" s="54"/>
       <c r="R67" s="1"/>
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
@@ -5725,10 +5732,10 @@
     </row>
     <row r="68" spans="2:21" ht="15" x14ac:dyDescent="0.2">
       <c r="B68" s="16"/>
-      <c r="C68" s="57"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="57"/>
-      <c r="F68" s="58"/>
+      <c r="C68" s="55"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="56"/>
       <c r="G68" s="44"/>
       <c r="H68" s="42"/>
       <c r="I68" s="45"/>
@@ -5738,8 +5745,8 @@
       <c r="M68" s="44"/>
       <c r="N68" s="42"/>
       <c r="O68" s="45"/>
-      <c r="P68" s="70"/>
-      <c r="Q68" s="71"/>
+      <c r="P68" s="53"/>
+      <c r="Q68" s="54"/>
       <c r="R68" s="1"/>
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
@@ -5747,10 +5754,10 @@
     </row>
     <row r="69" spans="2:21" ht="15" x14ac:dyDescent="0.2">
       <c r="B69" s="16"/>
-      <c r="C69" s="57"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="57"/>
-      <c r="F69" s="58"/>
+      <c r="C69" s="55"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="55"/>
+      <c r="F69" s="56"/>
       <c r="G69" s="44"/>
       <c r="H69" s="42"/>
       <c r="I69" s="45"/>
@@ -5760,8 +5767,8 @@
       <c r="M69" s="44"/>
       <c r="N69" s="42"/>
       <c r="O69" s="45"/>
-      <c r="P69" s="70"/>
-      <c r="Q69" s="71"/>
+      <c r="P69" s="53"/>
+      <c r="Q69" s="54"/>
       <c r="R69" s="1"/>
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
@@ -5769,10 +5776,10 @@
     </row>
     <row r="70" spans="2:21" ht="15" x14ac:dyDescent="0.2">
       <c r="B70" s="16"/>
-      <c r="C70" s="57"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="57"/>
-      <c r="F70" s="58"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="56"/>
       <c r="G70" s="44"/>
       <c r="H70" s="42"/>
       <c r="I70" s="45"/>
@@ -5782,8 +5789,8 @@
       <c r="M70" s="44"/>
       <c r="N70" s="42"/>
       <c r="O70" s="45"/>
-      <c r="P70" s="70"/>
-      <c r="Q70" s="71"/>
+      <c r="P70" s="53"/>
+      <c r="Q70" s="54"/>
       <c r="R70" s="1"/>
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
@@ -5791,10 +5798,10 @@
     </row>
     <row r="71" spans="2:21" ht="15" x14ac:dyDescent="0.2">
       <c r="B71" s="16"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="58"/>
+      <c r="C71" s="55"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="55"/>
+      <c r="F71" s="56"/>
       <c r="G71" s="44"/>
       <c r="H71" s="42"/>
       <c r="I71" s="45"/>
@@ -5804,8 +5811,8 @@
       <c r="M71" s="44"/>
       <c r="N71" s="42"/>
       <c r="O71" s="45"/>
-      <c r="P71" s="70"/>
-      <c r="Q71" s="71"/>
+      <c r="P71" s="53"/>
+      <c r="Q71" s="54"/>
       <c r="R71" s="1"/>
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
@@ -5813,10 +5820,10 @@
     </row>
     <row r="72" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="16"/>
-      <c r="C72" s="72"/>
-      <c r="D72" s="73"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="73"/>
+      <c r="C72" s="49"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="50"/>
       <c r="G72" s="46"/>
       <c r="H72" s="47"/>
       <c r="I72" s="48"/>
@@ -5826,8 +5833,8 @@
       <c r="M72" s="46"/>
       <c r="N72" s="47"/>
       <c r="O72" s="48"/>
-      <c r="P72" s="74"/>
-      <c r="Q72" s="75"/>
+      <c r="P72" s="51"/>
+      <c r="Q72" s="52"/>
       <c r="R72" s="1"/>
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
@@ -5835,10 +5842,10 @@
     </row>
     <row r="73" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B73" s="16"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="72"/>
-      <c r="F73" s="73"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="50"/>
       <c r="G73" s="46"/>
       <c r="H73" s="47"/>
       <c r="I73" s="48"/>
@@ -5848,8 +5855,8 @@
       <c r="M73" s="46"/>
       <c r="N73" s="47"/>
       <c r="O73" s="48"/>
-      <c r="P73" s="74"/>
-      <c r="Q73" s="75"/>
+      <c r="P73" s="51"/>
+      <c r="Q73" s="52"/>
       <c r="R73" s="1"/>
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
@@ -5857,10 +5864,10 @@
     </row>
     <row r="74" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="16"/>
-      <c r="C74" s="72"/>
-      <c r="D74" s="73"/>
-      <c r="E74" s="72"/>
-      <c r="F74" s="73"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="50"/>
       <c r="G74" s="46"/>
       <c r="H74" s="47"/>
       <c r="I74" s="48"/>
@@ -5870,16 +5877,16 @@
       <c r="M74" s="46"/>
       <c r="N74" s="47"/>
       <c r="O74" s="48"/>
-      <c r="P74" s="74"/>
-      <c r="Q74" s="75"/>
+      <c r="P74" s="51"/>
+      <c r="Q74" s="52"/>
       <c r="U74" s="17"/>
     </row>
     <row r="75" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B75" s="16"/>
-      <c r="C75" s="72"/>
-      <c r="D75" s="73"/>
-      <c r="E75" s="72"/>
-      <c r="F75" s="73"/>
+      <c r="C75" s="49"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="49"/>
+      <c r="F75" s="50"/>
       <c r="G75" s="46"/>
       <c r="H75" s="47"/>
       <c r="I75" s="48"/>
@@ -5889,16 +5896,16 @@
       <c r="M75" s="46"/>
       <c r="N75" s="47"/>
       <c r="O75" s="48"/>
-      <c r="P75" s="74"/>
-      <c r="Q75" s="75"/>
+      <c r="P75" s="51"/>
+      <c r="Q75" s="52"/>
       <c r="U75" s="17"/>
     </row>
     <row r="76" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="16"/>
-      <c r="C76" s="72"/>
-      <c r="D76" s="73"/>
-      <c r="E76" s="72"/>
-      <c r="F76" s="73"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="50"/>
       <c r="G76" s="46"/>
       <c r="H76" s="47"/>
       <c r="I76" s="48"/>
@@ -5908,16 +5915,16 @@
       <c r="M76" s="46"/>
       <c r="N76" s="47"/>
       <c r="O76" s="48"/>
-      <c r="P76" s="74"/>
-      <c r="Q76" s="75"/>
+      <c r="P76" s="51"/>
+      <c r="Q76" s="52"/>
       <c r="U76" s="17"/>
     </row>
     <row r="77" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B77" s="16"/>
-      <c r="C77" s="72"/>
-      <c r="D77" s="73"/>
-      <c r="E77" s="72"/>
-      <c r="F77" s="73"/>
+      <c r="C77" s="49"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="49"/>
+      <c r="F77" s="50"/>
       <c r="G77" s="46"/>
       <c r="H77" s="47"/>
       <c r="I77" s="48"/>
@@ -5927,16 +5934,16 @@
       <c r="M77" s="46"/>
       <c r="N77" s="47"/>
       <c r="O77" s="48"/>
-      <c r="P77" s="74"/>
-      <c r="Q77" s="75"/>
+      <c r="P77" s="51"/>
+      <c r="Q77" s="52"/>
       <c r="U77" s="17"/>
     </row>
     <row r="78" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="16"/>
-      <c r="C78" s="72"/>
-      <c r="D78" s="73"/>
-      <c r="E78" s="72"/>
-      <c r="F78" s="73"/>
+      <c r="C78" s="49"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="49"/>
+      <c r="F78" s="50"/>
       <c r="G78" s="46"/>
       <c r="H78" s="47"/>
       <c r="I78" s="48"/>
@@ -5946,16 +5953,16 @@
       <c r="M78" s="46"/>
       <c r="N78" s="47"/>
       <c r="O78" s="48"/>
-      <c r="P78" s="74"/>
-      <c r="Q78" s="75"/>
+      <c r="P78" s="51"/>
+      <c r="Q78" s="52"/>
       <c r="U78" s="17"/>
     </row>
     <row r="79" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="16"/>
-      <c r="C79" s="72"/>
-      <c r="D79" s="73"/>
-      <c r="E79" s="72"/>
-      <c r="F79" s="73"/>
+      <c r="C79" s="49"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="49"/>
+      <c r="F79" s="50"/>
       <c r="G79" s="46"/>
       <c r="H79" s="47"/>
       <c r="I79" s="48"/>
@@ -5965,148 +5972,252 @@
       <c r="M79" s="46"/>
       <c r="N79" s="47"/>
       <c r="O79" s="48"/>
-      <c r="P79" s="74"/>
-      <c r="Q79" s="75"/>
+      <c r="P79" s="51"/>
+      <c r="Q79" s="52"/>
       <c r="U79" s="17"/>
     </row>
-    <row r="80" spans="2:21" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:21" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="16"/>
+      <c r="C80" s="49"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="49"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="46"/>
+      <c r="H80" s="47"/>
+      <c r="I80" s="48"/>
+      <c r="J80" s="46"/>
+      <c r="K80" s="47"/>
+      <c r="L80" s="48"/>
+      <c r="M80" s="46"/>
+      <c r="N80" s="47"/>
+      <c r="O80" s="48"/>
+      <c r="P80" s="51"/>
+      <c r="Q80" s="52"/>
       <c r="U80" s="17"/>
     </row>
-    <row r="81" spans="2:21" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="38"/>
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
-      <c r="F81" s="39"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="39"/>
-      <c r="I81" s="39"/>
-      <c r="J81" s="39"/>
-      <c r="K81" s="39"/>
-      <c r="L81" s="39"/>
-      <c r="M81" s="39"/>
-      <c r="N81" s="39"/>
-      <c r="O81" s="39"/>
-      <c r="P81" s="39"/>
-      <c r="Q81" s="39"/>
-      <c r="R81" s="39"/>
-      <c r="S81" s="39"/>
-      <c r="T81" s="39"/>
-      <c r="U81" s="40"/>
-    </row>
-    <row r="82" spans="2:21" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="16"/>
+      <c r="C81" s="49"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="49"/>
+      <c r="F81" s="50"/>
+      <c r="G81" s="46"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="48"/>
+      <c r="J81" s="46"/>
+      <c r="K81" s="47"/>
+      <c r="L81" s="48"/>
+      <c r="M81" s="46"/>
+      <c r="N81" s="47"/>
+      <c r="O81" s="48"/>
+      <c r="P81" s="51"/>
+      <c r="Q81" s="52"/>
+      <c r="U81" s="17"/>
+    </row>
+    <row r="82" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="16"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="50"/>
+      <c r="G82" s="46"/>
+      <c r="H82" s="47"/>
+      <c r="I82" s="48"/>
+      <c r="J82" s="46"/>
+      <c r="K82" s="47"/>
+      <c r="L82" s="48"/>
+      <c r="M82" s="46"/>
+      <c r="N82" s="47"/>
+      <c r="O82" s="48"/>
+      <c r="P82" s="51"/>
+      <c r="Q82" s="52"/>
+      <c r="U82" s="17"/>
+    </row>
+    <row r="83" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="16"/>
+      <c r="C83" s="49"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="49"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="46"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="48"/>
+      <c r="J83" s="46"/>
+      <c r="K83" s="47"/>
+      <c r="L83" s="48"/>
+      <c r="M83" s="46"/>
+      <c r="N83" s="47"/>
+      <c r="O83" s="48"/>
+      <c r="P83" s="51"/>
+      <c r="Q83" s="52"/>
+      <c r="U83" s="17"/>
+    </row>
+    <row r="84" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="16"/>
+      <c r="C84" s="49"/>
+      <c r="D84" s="50"/>
+      <c r="E84" s="49"/>
+      <c r="F84" s="50"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="48"/>
+      <c r="J84" s="46"/>
+      <c r="K84" s="47"/>
+      <c r="L84" s="48"/>
+      <c r="M84" s="46"/>
+      <c r="N84" s="47"/>
+      <c r="O84" s="48"/>
+      <c r="P84" s="51"/>
+      <c r="Q84" s="52"/>
+      <c r="U84" s="17"/>
+    </row>
+    <row r="85" spans="2:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="16"/>
+      <c r="C85" s="49"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="49"/>
+      <c r="F85" s="50"/>
+      <c r="G85" s="46"/>
+      <c r="H85" s="47"/>
+      <c r="I85" s="48"/>
+      <c r="J85" s="46"/>
+      <c r="K85" s="47"/>
+      <c r="L85" s="48"/>
+      <c r="M85" s="46"/>
+      <c r="N85" s="47"/>
+      <c r="O85" s="48"/>
+      <c r="P85" s="51"/>
+      <c r="Q85" s="52"/>
+      <c r="U85" s="17"/>
+      <c r="Y85" s="76"/>
+    </row>
+    <row r="86" spans="2:25" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="16"/>
+      <c r="U86" s="17"/>
+    </row>
+    <row r="87" spans="2:25" ht="21.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="38"/>
+      <c r="C87" s="39"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="39"/>
+      <c r="F87" s="39"/>
+      <c r="G87" s="39"/>
+      <c r="H87" s="39"/>
+      <c r="I87" s="39"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="39"/>
+      <c r="L87" s="39"/>
+      <c r="M87" s="39"/>
+      <c r="N87" s="39"/>
+      <c r="O87" s="39"/>
+      <c r="P87" s="39"/>
+      <c r="Q87" s="39"/>
+      <c r="R87" s="39"/>
+      <c r="S87" s="39"/>
+      <c r="T87" s="39"/>
+      <c r="U87" s="40"/>
+    </row>
+    <row r="88" spans="2:25" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="213">
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="P79:Q79"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="P77:Q77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="P78:Q78"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="P74:Q74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="P75:Q75"/>
-    <mergeCell ref="P71:Q71"/>
-    <mergeCell ref="P72:Q72"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="P63:Q63"/>
-    <mergeCell ref="P64:Q64"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="P53:Q53"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="P60:Q60"/>
-    <mergeCell ref="P61:Q61"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="P51:Q51"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
+  <mergeCells count="231">
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="P84:Q84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="E80:F80"/>
+    <mergeCell ref="P80:Q80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="P81:Q81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="E82:F82"/>
+    <mergeCell ref="P82:Q82"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P12:Q13"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B6:U6"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
@@ -6131,86 +6242,115 @@
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
     <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B6:U6"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="E12:F13"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P12:Q13"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B2:U2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:P5"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="P60:Q60"/>
+    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="P71:Q71"/>
+    <mergeCell ref="P72:Q72"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="P63:Q63"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="P70:Q70"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="P74:Q74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="P79:Q79"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="P77:Q77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="P78:Q78"/>
   </mergeCells>
   <pageMargins left="1.299212598425197" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="45" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>